<commit_message>
update logs and project plan
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1D5458-7443-440F-B93A-1CF0CB13F675}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B9EA81-61B1-4433-85A1-B9B0F1AB0BA7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Week</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>presentation!!!   &amp; AWS!!!</t>
+  </si>
+  <si>
+    <t>Team Project setup</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,13 +719,28 @@
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1.5</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Store entity complete. Item entity started
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B9EA81-61B1-4433-85A1-B9B0F1AB0BA7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8579430-7A91-483C-BF72-7D172B0C92E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Week</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Team Project setup</t>
+  </si>
+  <si>
+    <t>Team Project work</t>
   </si>
 </sst>
 </file>
@@ -454,13 +457,13 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
@@ -747,13 +750,25 @@
       <c r="A12" t="s">
         <v>16</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <v>3.75</v>
+      </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
all tests pass, together
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA2F056-8BD3-4004-B243-CAD530915FD8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D4D5C5-B6F5-4DB8-AD6C-6BEA43034F9A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -798,7 +798,7 @@
         <v>18</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
@@ -806,7 +806,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
shoppingList entity and daoTests done.  logs updated
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6815A91-6655-44F1-9AC4-21C652EE4C2C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C252D3F-5686-47EE-8286-90F0AD3D0FF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -798,7 +798,7 @@
         <v>18</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
@@ -806,7 +806,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working to display user with role - need to annotate user
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C252D3F-5686-47EE-8286-90F0AD3D0FF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E1EB3E-018A-4251-85D8-FC21B130164E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,16 +797,19 @@
       <c r="A14" t="s">
         <v>18</v>
       </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
       <c r="F14">
-        <v>4.75</v>
+        <v>6.75</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lombok toString, hash & dotEquals -> tests passing
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D70CF0-C15D-47C6-A0B8-E304FE7A35E7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4177AA81-6E7E-4A62-80D3-11F6F5F3B6C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,13 +819,16 @@
       <c r="A15" t="s">
         <v>19</v>
       </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
       <c r="G15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated logs with non-intelliJ UI work
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9EAA65-656B-471A-8FBC-5CD91F4FB398}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9E5F61-F832-4AFE-A84C-4F060B9B0D15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Week</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Team Project work</t>
+  </si>
+  <si>
+    <t>3 hours code review</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,16 +822,22 @@
       <c r="A15" t="s">
         <v>19</v>
       </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
       <c r="F15">
-        <v>3.5</v>
+        <v>8</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
conditional showing of table headers - done
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E9AD4A-0481-4AE1-B0BC-36758860504C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EAC6E0-9AF2-46ED-BBC7-3CF9A7CA35A8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,7 +826,7 @@
         <v>3</v>
       </c>
       <c r="F15">
-        <v>16.25</v>
+        <v>20.25</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>23.25</v>
       </c>
       <c r="I15" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
jquery datatables added to js file
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EAC6E0-9AF2-46ED-BBC7-3CF9A7CA35A8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1894A42A-FA63-4288-924F-7250AF72F822}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,7 +826,7 @@
         <v>3</v>
       </c>
       <c r="F15">
-        <v>20.25</v>
+        <v>23.75</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>23.25</v>
+        <v>26.75</v>
       </c>
       <c r="I15" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
built deal search form, minus ajax fill of select options from db
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDDF2EB-BCFE-4393-9F35-6C5F411C7C8F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E654924A-50F1-4394-99D3-35EE81B58F2E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="F16">
-        <v>11.5</v>
+        <v>14.5</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>11.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
all tests updated to pass, with category
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF002B6-38E0-4439-9960-0E3E5D8B9DAA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50439FD0-08B3-4646-8A13-C9BD1B911ADF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="F16">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
user delete and update (role, pwd) working
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA3895F-B00D-49D3-B394-EF1E0B675E0F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B58AF9B-8D0C-42D9-B465-A2B2210AA8C7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="F16">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
beginning user edit my info form
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D3B752-BA5A-4D51-A3D4-24B0E9653CB8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94348ECE-B4EF-4009-8B57-B94EAF440628}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="F16">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated logs, uploaded videos to youtube, added links to readme
</commit_message>
<xml_diff>
--- a/EntJava_classHrs.xlsx
+++ b/EntJava_classHrs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rica\IdeaProjects\grocerySales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94348ECE-B4EF-4009-8B57-B94EAF440628}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E700A3D-806B-4DBF-B7C4-1DC51BB6559F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="F16">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>